<commit_message>
fix radio sound bug
</commit_message>
<xml_diff>
--- a/core/assets/levels/tut0.xlsx
+++ b/core/assets/levels/tut0.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Program Files\Git\MangoSnoopers\core\assets\levels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{252A2C32-1A7A-4266-8D54-64DE2DF68259}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E2E3EEC-E91C-4418-8C07-637C7D90FC75}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7680" yWindow="0" windowWidth="15240" windowHeight="6660" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8625" yWindow="0" windowWidth="15240" windowHeight="6660" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="46">
   <si>
     <t>Region</t>
   </si>
@@ -718,7 +718,7 @@
   <dimension ref="A1:AS1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.125" defaultRowHeight="15" customHeight="1"/>
@@ -1047,9 +1047,7 @@
       <c r="E19" s="2"/>
       <c r="F19" s="2"/>
       <c r="G19" s="5"/>
-      <c r="H19" s="5" t="s">
-        <v>9</v>
-      </c>
+      <c r="H19" s="5"/>
       <c r="I19" s="5"/>
       <c r="J19" s="2"/>
     </row>
@@ -1061,9 +1059,7 @@
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
       <c r="G20" s="5"/>
-      <c r="H20" s="5" t="s">
-        <v>9</v>
-      </c>
+      <c r="H20" s="5"/>
       <c r="I20" s="5"/>
       <c r="J20" s="2"/>
     </row>
@@ -1077,9 +1073,7 @@
       <c r="E21" s="2"/>
       <c r="F21" s="2"/>
       <c r="G21" s="5"/>
-      <c r="H21" s="2" t="s">
-        <v>9</v>
-      </c>
+      <c r="H21" s="2"/>
       <c r="I21" s="5"/>
       <c r="J21" s="2"/>
     </row>
@@ -1096,7 +1090,9 @@
       <c r="H22" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="I22" s="5"/>
+      <c r="I22" s="5" t="s">
+        <v>9</v>
+      </c>
       <c r="J22" s="2"/>
     </row>
     <row r="23" spans="1:45" ht="16.5" customHeight="1">

</xml_diff>

<commit_message>
narration in tut 0 lol
</commit_message>
<xml_diff>
--- a/core/assets/levels/tut0.xlsx
+++ b/core/assets/levels/tut0.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Program Files\Git\MangoSnoopers\core\assets\levels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E2E3EEC-E91C-4418-8C07-637C7D90FC75}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{419146E9-AF7C-49AA-9011-815220E566E5}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="8625" yWindow="0" windowWidth="15240" windowHeight="6660" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -718,7 +718,7 @@
   <dimension ref="A1:AS1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.125" defaultRowHeight="15" customHeight="1"/>
@@ -826,13 +826,6 @@
         <v>44</v>
       </c>
       <c r="D4" s="10"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="5"/>
-      <c r="H4" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="I4" s="5"/>
     </row>
     <row r="5" spans="1:10" ht="16.5" customHeight="1">
       <c r="A5">
@@ -845,11 +838,6 @@
         <v>0</v>
       </c>
       <c r="D5" s="10"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="5"/>
-      <c r="H5" s="3"/>
-      <c r="I5" s="5"/>
       <c r="J5" s="2"/>
     </row>
     <row r="6" spans="1:10" ht="16.5" customHeight="1">
@@ -857,11 +845,6 @@
       <c r="B6" s="10"/>
       <c r="C6" s="10"/>
       <c r="D6" s="10"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
-      <c r="H6" s="2"/>
-      <c r="I6" s="2"/>
       <c r="J6" s="2"/>
     </row>
     <row r="7" spans="1:10" ht="16.5" customHeight="1">
@@ -870,17 +853,6 @@
       </c>
       <c r="B7" s="10"/>
       <c r="C7" s="10"/>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
-      <c r="G7" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="H7" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="I7" s="2" t="s">
-        <v>9</v>
-      </c>
       <c r="J7" s="1"/>
     </row>
     <row r="8" spans="1:10" ht="16.5" customHeight="1">
@@ -892,53 +864,21 @@
       </c>
       <c r="C8" s="10"/>
       <c r="D8" s="10"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
-      <c r="G8" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="H8" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="I8" s="3" t="s">
-        <v>9</v>
-      </c>
       <c r="J8" s="2"/>
     </row>
     <row r="9" spans="1:10" ht="16.5" customHeight="1">
       <c r="C9" s="10"/>
       <c r="D9" s="10"/>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
-      <c r="G9" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="H9" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="I9" s="3" t="s">
-        <v>9</v>
-      </c>
       <c r="J9" s="2"/>
     </row>
     <row r="10" spans="1:10" ht="16.5" customHeight="1">
       <c r="C10" s="10"/>
       <c r="D10" s="10"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-      <c r="G10" s="2"/>
-      <c r="H10" s="2"/>
-      <c r="I10" s="2"/>
       <c r="J10" s="2"/>
     </row>
     <row r="11" spans="1:10" ht="16.5" customHeight="1">
       <c r="C11" s="10"/>
       <c r="D11" s="10"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
-      <c r="G11" s="3"/>
-      <c r="H11" s="3"/>
-      <c r="I11" s="3"/>
       <c r="J11" s="2"/>
     </row>
     <row r="12" spans="1:10" ht="16.5" customHeight="1">
@@ -946,11 +886,6 @@
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
-      <c r="G12" s="3"/>
-      <c r="H12" s="3"/>
-      <c r="I12" s="3"/>
       <c r="J12" s="2"/>
     </row>
     <row r="13" spans="1:10" ht="16.5" customHeight="1">
@@ -958,11 +893,6 @@
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
-      <c r="G13" s="5"/>
-      <c r="H13" s="5"/>
-      <c r="I13" s="5"/>
       <c r="J13" s="2"/>
     </row>
     <row r="14" spans="1:10" ht="16.5" customHeight="1">
@@ -970,11 +900,6 @@
       <c r="B14" s="6"/>
       <c r="C14" s="6"/>
       <c r="D14" s="6"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
-      <c r="G14" s="5"/>
-      <c r="H14" s="2"/>
-      <c r="I14" s="5"/>
       <c r="J14" s="2"/>
     </row>
     <row r="15" spans="1:10" ht="16.5" customHeight="1">
@@ -984,11 +909,6 @@
       <c r="B15" s="6"/>
       <c r="C15" s="6"/>
       <c r="D15" s="6"/>
-      <c r="E15" s="2"/>
-      <c r="F15" s="2"/>
-      <c r="G15" s="5"/>
-      <c r="H15" s="5"/>
-      <c r="I15" s="5"/>
       <c r="J15" s="2"/>
     </row>
     <row r="16" spans="1:10" ht="16.5" customHeight="1">
@@ -996,15 +916,6 @@
       <c r="B16" s="6"/>
       <c r="C16" s="6"/>
       <c r="D16" s="6"/>
-      <c r="E16" s="2"/>
-      <c r="F16" s="2"/>
-      <c r="G16" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="H16" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="I16" s="5"/>
       <c r="J16" s="2"/>
     </row>
     <row r="17" spans="1:45" ht="16.5" customHeight="1">
@@ -1012,13 +923,6 @@
       <c r="B17" s="6"/>
       <c r="C17" s="6"/>
       <c r="D17" s="6"/>
-      <c r="E17" s="2"/>
-      <c r="F17" s="2"/>
-      <c r="G17" s="5"/>
-      <c r="H17" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="I17" s="5"/>
       <c r="J17" s="2"/>
     </row>
     <row r="18" spans="1:45" ht="16.5" customHeight="1">
@@ -1028,10 +932,8 @@
       <c r="D18" s="6"/>
       <c r="E18" s="2"/>
       <c r="F18" s="2"/>
-      <c r="G18" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="H18" s="2" t="s">
+      <c r="G18" s="5"/>
+      <c r="H18" s="3" t="s">
         <v>9</v>
       </c>
       <c r="I18" s="5"/>
@@ -1047,7 +949,7 @@
       <c r="E19" s="2"/>
       <c r="F19" s="2"/>
       <c r="G19" s="5"/>
-      <c r="H19" s="5"/>
+      <c r="H19" s="3"/>
       <c r="I19" s="5"/>
       <c r="J19" s="2"/>
     </row>
@@ -1058,9 +960,9 @@
       <c r="D20" s="6"/>
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
-      <c r="G20" s="5"/>
-      <c r="H20" s="5"/>
-      <c r="I20" s="5"/>
+      <c r="G20" s="2"/>
+      <c r="H20" s="2"/>
+      <c r="I20" s="2"/>
       <c r="J20" s="2"/>
     </row>
     <row r="21" spans="1:45" ht="16.5" customHeight="1">
@@ -1070,11 +972,17 @@
       <c r="B21" s="6"/>
       <c r="C21" s="6"/>
       <c r="D21" s="6"/>
-      <c r="E21" s="2"/>
-      <c r="F21" s="2"/>
-      <c r="G21" s="5"/>
-      <c r="H21" s="2"/>
-      <c r="I21" s="5"/>
+      <c r="E21" s="1"/>
+      <c r="F21" s="1"/>
+      <c r="G21" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H21" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="I21" s="2" t="s">
+        <v>9</v>
+      </c>
       <c r="J21" s="2"/>
     </row>
     <row r="22" spans="1:45" ht="16.5" customHeight="1">
@@ -1086,11 +994,13 @@
       <c r="D22" s="6"/>
       <c r="E22" s="2"/>
       <c r="F22" s="2"/>
-      <c r="G22" s="5"/>
-      <c r="H22" s="2" t="s">
+      <c r="G22" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="I22" s="5" t="s">
+      <c r="H22" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I22" s="3" t="s">
         <v>9</v>
       </c>
       <c r="J22" s="2"/>
@@ -1104,11 +1014,15 @@
       <c r="D23" s="6"/>
       <c r="E23" s="2"/>
       <c r="F23" s="2"/>
-      <c r="G23" s="2"/>
-      <c r="H23" s="5" t="s">
+      <c r="G23" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="I23" s="2"/>
+      <c r="H23" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I23" s="3" t="s">
+        <v>9</v>
+      </c>
       <c r="J23" s="2"/>
     </row>
     <row r="24" spans="1:45" ht="16.5" customHeight="1">
@@ -1118,13 +1032,11 @@
       <c r="B24" s="6"/>
       <c r="C24" s="6"/>
       <c r="D24" s="6"/>
-      <c r="E24" s="2" t="s">
-        <v>22</v>
-      </c>
+      <c r="E24" s="2"/>
       <c r="F24" s="2"/>
       <c r="G24" s="2"/>
       <c r="H24" s="2"/>
-      <c r="I24" s="5"/>
+      <c r="I24" s="2"/>
       <c r="J24" s="2"/>
     </row>
     <row r="25" spans="1:45" ht="16.5" customHeight="1">
@@ -1136,9 +1048,9 @@
       <c r="D25" s="6"/>
       <c r="E25" s="2"/>
       <c r="F25" s="2"/>
-      <c r="G25" s="2"/>
-      <c r="H25" s="5"/>
-      <c r="I25" s="2"/>
+      <c r="G25" s="3"/>
+      <c r="H25" s="3"/>
+      <c r="I25" s="3"/>
       <c r="J25" s="2"/>
     </row>
     <row r="26" spans="1:45" ht="16.5" customHeight="1">
@@ -1148,9 +1060,11 @@
       <c r="B26" s="6"/>
       <c r="C26" s="6"/>
       <c r="D26" s="6"/>
-      <c r="G26" s="2"/>
-      <c r="H26" s="2"/>
-      <c r="I26" s="2"/>
+      <c r="E26" s="2"/>
+      <c r="F26" s="2"/>
+      <c r="G26" s="3"/>
+      <c r="H26" s="3"/>
+      <c r="I26" s="3"/>
       <c r="J26" s="1"/>
     </row>
     <row r="27" spans="1:45" ht="16.5" customHeight="1">
@@ -1160,6 +1074,11 @@
       <c r="B27" s="6"/>
       <c r="C27" s="6"/>
       <c r="D27" s="6"/>
+      <c r="E27" s="2"/>
+      <c r="F27" s="2"/>
+      <c r="G27" s="5"/>
+      <c r="H27" s="5"/>
+      <c r="I27" s="5"/>
       <c r="J27" s="1"/>
       <c r="K27" s="2"/>
       <c r="L27" s="2"/>
@@ -1170,8 +1089,11 @@
       <c r="B28" s="6"/>
       <c r="C28" s="6"/>
       <c r="D28" s="6"/>
-      <c r="E28" s="1"/>
-      <c r="F28" s="1"/>
+      <c r="E28" s="2"/>
+      <c r="F28" s="2"/>
+      <c r="G28" s="5"/>
+      <c r="H28" s="2"/>
+      <c r="I28" s="5"/>
       <c r="J28" s="1"/>
       <c r="K28" s="2"/>
       <c r="L28" s="2"/>
@@ -1184,6 +1106,11 @@
       <c r="B29" s="6"/>
       <c r="C29" s="6"/>
       <c r="D29" s="6"/>
+      <c r="E29" s="2"/>
+      <c r="F29" s="2"/>
+      <c r="G29" s="5"/>
+      <c r="H29" s="5"/>
+      <c r="I29" s="5"/>
       <c r="J29" s="2"/>
       <c r="K29" s="2"/>
       <c r="L29" s="2"/>
@@ -1196,6 +1123,15 @@
       <c r="B30" s="6"/>
       <c r="C30" s="6"/>
       <c r="D30" s="6"/>
+      <c r="E30" s="2"/>
+      <c r="F30" s="2"/>
+      <c r="G30" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="H30" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I30" s="5"/>
       <c r="J30" s="2"/>
       <c r="K30" s="2"/>
       <c r="L30" s="2"/>
@@ -1208,6 +1144,13 @@
       <c r="B31" s="6"/>
       <c r="C31" s="6"/>
       <c r="D31" s="6"/>
+      <c r="E31" s="2"/>
+      <c r="F31" s="2"/>
+      <c r="G31" s="5"/>
+      <c r="H31" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="I31" s="5"/>
       <c r="J31" s="2"/>
       <c r="K31" s="2"/>
       <c r="L31" s="2"/>
@@ -1220,6 +1163,15 @@
       <c r="B32" s="6"/>
       <c r="C32" s="6"/>
       <c r="D32" s="6"/>
+      <c r="E32" s="2"/>
+      <c r="F32" s="2"/>
+      <c r="G32" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="H32" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="I32" s="5"/>
       <c r="J32" s="2"/>
       <c r="K32" s="2"/>
       <c r="L32" s="2"/>
@@ -1264,6 +1216,11 @@
       <c r="B33" s="6"/>
       <c r="C33" s="6"/>
       <c r="D33" s="6"/>
+      <c r="E33" s="2"/>
+      <c r="F33" s="2"/>
+      <c r="G33" s="5"/>
+      <c r="H33" s="5"/>
+      <c r="I33" s="5"/>
       <c r="J33" s="2"/>
       <c r="K33" s="2"/>
       <c r="L33" s="2"/>
@@ -1306,6 +1263,11 @@
       <c r="B34" s="6"/>
       <c r="C34" s="6"/>
       <c r="D34" s="6"/>
+      <c r="E34" s="2"/>
+      <c r="F34" s="2"/>
+      <c r="G34" s="5"/>
+      <c r="H34" s="5"/>
+      <c r="I34" s="5"/>
       <c r="J34" s="2"/>
       <c r="K34" s="2"/>
       <c r="L34" s="2"/>
@@ -1350,6 +1312,11 @@
       <c r="B35" s="6"/>
       <c r="C35" s="6"/>
       <c r="D35" s="6"/>
+      <c r="E35" s="2"/>
+      <c r="F35" s="2"/>
+      <c r="G35" s="5"/>
+      <c r="H35" s="2"/>
+      <c r="I35" s="5"/>
       <c r="J35" s="2"/>
       <c r="K35" s="2"/>
       <c r="L35" s="2"/>
@@ -1394,6 +1361,15 @@
       <c r="B36" s="6"/>
       <c r="C36" s="6"/>
       <c r="D36" s="6"/>
+      <c r="E36" s="2"/>
+      <c r="F36" s="2"/>
+      <c r="G36" s="5"/>
+      <c r="H36" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="I36" s="5" t="s">
+        <v>9</v>
+      </c>
       <c r="J36" s="2"/>
       <c r="K36" s="2"/>
       <c r="L36" s="2"/>
@@ -1438,6 +1414,13 @@
       <c r="B37" s="6"/>
       <c r="C37" s="6"/>
       <c r="D37" s="6"/>
+      <c r="E37" s="2"/>
+      <c r="F37" s="2"/>
+      <c r="G37" s="2"/>
+      <c r="H37" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="I37" s="2"/>
       <c r="J37" s="2"/>
       <c r="K37" s="2"/>
       <c r="L37" s="2"/>
@@ -1482,6 +1465,13 @@
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
       <c r="D38" s="6"/>
+      <c r="E38" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="F38" s="2"/>
+      <c r="G38" s="2"/>
+      <c r="H38" s="2"/>
+      <c r="I38" s="5"/>
       <c r="J38" s="2"/>
       <c r="K38" s="2"/>
       <c r="L38" s="2"/>
@@ -46683,6 +46673,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
-  <pageSetup orientation="landscape"/>
+  <pageSetup orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
making the jar work
</commit_message>
<xml_diff>
--- a/core/assets/levels/tut0.xlsx
+++ b/core/assets/levels/tut0.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Program Files\Git\MangoSnoopers\core\assets\levels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{419146E9-AF7C-49AA-9011-815220E566E5}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E539FB1-9F1A-4676-BA37-DD34BA3E2F87}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8625" yWindow="0" windowWidth="15240" windowHeight="6660" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="945" yWindow="0" windowWidth="27855" windowHeight="12810" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>

</xml_diff>